<commit_message>
added BOM and STL to leson 1
</commit_message>
<xml_diff>
--- a/L1 - Arduino Robot Arm/BOM.xlsx
+++ b/L1 - Arduino Robot Arm/BOM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MEGAsync\RobotMind\Channel\arduinobot\arduinobot-tutorial\L1 - Arduino Robot Arm\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DA5F19-E7E9-4DC1-A8FF-DF41F455F286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Arduino UNO</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3/4 or PC</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Power Supply Module</t>
+  </si>
+  <si>
+    <t>Prototype Expansion Board</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M3 Screws and Nuts</t>
+  </si>
+  <si>
+    <t>SG90 servo motors (x4)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,13 +93,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +159,323 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3657600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2459354</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Immagine 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70846EAC-3C6E-48A2-9161-CA2918413950}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2533651" y="219075"/>
+          <a:ext cx="3638549" cy="2430779"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3676650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2526286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Immagine 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90C5F36E-ADC7-4F64-9906-2BFC541C7A84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524125" y="2676526"/>
+          <a:ext cx="3667125" cy="2516760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3124200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2743200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Immagine 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C760FAF1-CBAE-4D66-9A1D-DF6CAAF926C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2924175" y="5267325"/>
+          <a:ext cx="2714625" cy="2714625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>681773</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2771775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1961046</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Immagine 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C5B199-D472-40AA-A8C4-F8F6B0CA2534}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3196373" y="8029574"/>
+          <a:ext cx="2090002" cy="1941997"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3448050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3429000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Immagine 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4163CA1B-34AA-470E-BB54-1B8611DB6A1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2571750" y="10058400"/>
+          <a:ext cx="3390900" cy="3390900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>48958</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3171825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2293430</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Immagine 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{404E5AAC-7585-47BD-978F-D1A8F79DDD40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3286124" y="13564933"/>
+          <a:ext cx="2609851" cy="2244472"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DCC6B52D-B0C5-406C-8DDA-C855E1D3ADF1}" name="Tabella1" displayName="Tabella1" ref="A1:C7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="4">
+  <autoFilter ref="A1:C7" xr:uid="{DF937480-ABE4-4A2B-92F8-74A071E74EC0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{98935867-2975-48C9-B7CA-419B021ACDB4}" name="Product" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{835EABB7-A6D7-4CEA-9AEF-C02DCACC163E}" name="Required" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D6BAB1E8-6EA4-4360-82C4-CE38C957A8D3}" name="Image" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +740,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="275.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="189" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>